<commit_message>
Update Excel Table data for project.xlsx
Updated the work for the data tables as I continue the project.
</commit_message>
<xml_diff>
--- a/Computer_Science_CS/4700_Database_Management/Excel Table data for project.xlsx
+++ b/Computer_Science_CS/4700_Database_Management/Excel Table data for project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CWF\GitHub\College_Courses\Computer_Science_CS\4700_Database_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C01F183-6855-4B5C-B745-E015F36C4448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191AEC54-3922-4FD9-B616-A046A7C11C2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{4BA7C107-2613-45E6-9465-717CD4711F58}"/>
   </bookViews>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825E227C-D05A-4E33-AE3F-27BCBFCD53C6}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>2116713492</v>
+        <v>9731265483</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <v>7649803654</v>
+        <v>9986431026</v>
       </c>
       <c r="B33">
         <v>9</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <v>7649803654</v>
+        <v>9986431026</v>
       </c>
       <c r="B35">
         <v>7</v>

</xml_diff>